<commit_message>
cambios iconos en ui y nuevas gráficas en server
</commit_message>
<xml_diff>
--- a/app-medicine-r/modulos/data/datos_supensiones_por_especialidad.xlsx
+++ b/app-medicine-r/modulos/data/datos_supensiones_por_especialidad.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\app_health_r_medicine\app-mvp\modulos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\app_health_r_medicine\app-medicine-r\modulos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBA7F3A-175E-43F7-8772-6BB5385F64BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16F9EE7-C0B7-4D36-80FE-9229A38E8443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{109DEA4C-15FF-477D-B494-C4225E7A906B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="32">
   <si>
     <t>Especialidad</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Urología</t>
   </si>
   <si>
-    <t>Cirugí digestiva alta</t>
-  </si>
-  <si>
     <t>Cirugía infantil</t>
   </si>
   <si>
@@ -129,6 +126,12 @@
   </si>
   <si>
     <t>cantidad</t>
+  </si>
+  <si>
+    <t>Cirugía digestiva alta</t>
+  </si>
+  <si>
+    <t>cirugía digestiva alta</t>
   </si>
 </sst>
 </file>
@@ -482,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05386F-DCE1-46E7-9BA0-AADCBB94F0A3}">
   <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="L73" sqref="L73"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="93" workbookViewId="0">
+      <selection activeCell="M84" sqref="M84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,22 +516,22 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
-        <v>27</v>
-      </c>
       <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" t="s">
         <v>29</v>
-      </c>
-      <c r="N1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -553,7 +556,7 @@
         <v/>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -586,7 +589,7 @@
         <v>68</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
         <v>1</v>
@@ -622,7 +625,7 @@
         <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
@@ -658,7 +661,7 @@
         <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
         <v>3</v>
@@ -694,7 +697,7 @@
         <v>30</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J6" t="s">
         <v>4</v>
@@ -747,7 +750,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>20</v>
@@ -775,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="O8">
         <v>20</v>
@@ -783,7 +786,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>13</v>
@@ -811,7 +814,7 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O9">
         <v>13</v>
@@ -819,7 +822,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>12</v>
@@ -844,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O10">
         <v>12</v>
@@ -852,7 +855,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -880,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O11">
         <v>9</v>
@@ -888,7 +891,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -910,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O12">
         <v>4</v>
@@ -918,7 +921,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -934,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K13">
         <v>20</v>
@@ -943,7 +946,7 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O13">
         <v>4</v>
@@ -951,7 +954,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -967,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K14">
         <v>13</v>
@@ -976,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O14">
         <v>3</v>
@@ -984,7 +987,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -997,7 +1000,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K15">
         <v>12</v>
@@ -1006,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O15">
         <v>1</v>
@@ -1014,16 +1017,20 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <v>6</v>
       </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="I16" t="s">
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K16">
         <v>9</v>
@@ -1032,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -1040,7 +1047,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1053,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K17">
         <v>4</v>
@@ -1062,7 +1069,7 @@
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1070,7 +1077,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -1083,7 +1090,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K18">
         <v>4</v>
@@ -1092,7 +1099,7 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1100,7 +1107,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1113,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K19">
         <v>3</v>
@@ -1122,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1130,7 +1137,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <f>SUM(B2:B19)</f>
@@ -1156,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -1176,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -1196,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -1216,7 +1223,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -1236,7 +1243,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -1285,7 +1292,7 @@
         <v>2</v>
       </c>
       <c r="N26" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1305,7 +1312,7 @@
         <v>2</v>
       </c>
       <c r="N27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O27">
         <v>2</v>
@@ -1325,7 +1332,7 @@
         <v>2</v>
       </c>
       <c r="N28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O28">
         <v>0</v>
@@ -1345,7 +1352,7 @@
         <v>2</v>
       </c>
       <c r="N29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O29">
         <v>1</v>
@@ -1365,7 +1372,7 @@
         <v>2</v>
       </c>
       <c r="N30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O30">
         <v>0</v>
@@ -1376,7 +1383,7 @@
         <v>2</v>
       </c>
       <c r="J31" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -1385,7 +1392,7 @@
         <v>2</v>
       </c>
       <c r="N31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O31">
         <v>21</v>
@@ -1396,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="J32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K32">
         <v>2</v>
@@ -1405,7 +1412,7 @@
         <v>2</v>
       </c>
       <c r="N32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O32">
         <v>0</v>
@@ -1416,7 +1423,7 @@
         <v>2</v>
       </c>
       <c r="J33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -1425,7 +1432,7 @@
         <v>2</v>
       </c>
       <c r="N33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O33">
         <v>0</v>
@@ -1436,7 +1443,7 @@
         <v>2</v>
       </c>
       <c r="J34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K34">
         <v>1</v>
@@ -1445,7 +1452,7 @@
         <v>2</v>
       </c>
       <c r="N34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O34">
         <v>0</v>
@@ -1456,7 +1463,7 @@
         <v>2</v>
       </c>
       <c r="J35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -1465,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="N35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O35">
         <v>0</v>
@@ -1476,7 +1483,7 @@
         <v>2</v>
       </c>
       <c r="J36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K36">
         <v>21</v>
@@ -1485,7 +1492,7 @@
         <v>2</v>
       </c>
       <c r="N36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -1496,7 +1503,7 @@
         <v>2</v>
       </c>
       <c r="J37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -1505,7 +1512,7 @@
         <v>2</v>
       </c>
       <c r="N37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O37">
         <v>2</v>
@@ -1516,7 +1523,7 @@
         <v>2</v>
       </c>
       <c r="J38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -1536,7 +1543,7 @@
         <v>2</v>
       </c>
       <c r="J39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -1556,7 +1563,7 @@
         <v>2</v>
       </c>
       <c r="J40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -1576,7 +1583,7 @@
         <v>2</v>
       </c>
       <c r="J41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -1596,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="J42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K42">
         <v>2</v>
@@ -1645,7 +1652,7 @@
         <v>3</v>
       </c>
       <c r="N44" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="O44">
         <v>2</v>
@@ -1665,7 +1672,7 @@
         <v>3</v>
       </c>
       <c r="N45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O45">
         <v>0</v>
@@ -1685,7 +1692,7 @@
         <v>3</v>
       </c>
       <c r="N46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -1705,7 +1712,7 @@
         <v>3</v>
       </c>
       <c r="N47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O47">
         <v>0</v>
@@ -1725,7 +1732,7 @@
         <v>3</v>
       </c>
       <c r="N48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O48">
         <v>0</v>
@@ -1736,7 +1743,7 @@
         <v>3</v>
       </c>
       <c r="J49" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="K49">
         <v>2</v>
@@ -1745,7 +1752,7 @@
         <v>3</v>
       </c>
       <c r="N49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O49">
         <v>0</v>
@@ -1756,7 +1763,7 @@
         <v>3</v>
       </c>
       <c r="J50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K50">
         <v>0</v>
@@ -1765,7 +1772,7 @@
         <v>3</v>
       </c>
       <c r="N50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O50">
         <v>0</v>
@@ -1776,7 +1783,7 @@
         <v>3</v>
       </c>
       <c r="J51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K51">
         <v>0</v>
@@ -1785,7 +1792,7 @@
         <v>3</v>
       </c>
       <c r="N51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O51">
         <v>0</v>
@@ -1796,7 +1803,7 @@
         <v>3</v>
       </c>
       <c r="J52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K52">
         <v>0</v>
@@ -1805,7 +1812,7 @@
         <v>3</v>
       </c>
       <c r="N52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O52">
         <v>0</v>
@@ -1816,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="J53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -1825,7 +1832,7 @@
         <v>3</v>
       </c>
       <c r="N53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O53">
         <v>0</v>
@@ -1836,7 +1843,7 @@
         <v>3</v>
       </c>
       <c r="J54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K54">
         <v>0</v>
@@ -1845,7 +1852,7 @@
         <v>3</v>
       </c>
       <c r="N54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O54">
         <v>0</v>
@@ -1856,7 +1863,7 @@
         <v>3</v>
       </c>
       <c r="J55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K55">
         <v>0</v>
@@ -1865,7 +1872,7 @@
         <v>3</v>
       </c>
       <c r="N55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O55">
         <v>0</v>
@@ -1876,7 +1883,7 @@
         <v>3</v>
       </c>
       <c r="J56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K56">
         <v>0</v>
@@ -1896,7 +1903,7 @@
         <v>3</v>
       </c>
       <c r="J57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -1916,7 +1923,7 @@
         <v>3</v>
       </c>
       <c r="J58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K58">
         <v>0</v>
@@ -1936,7 +1943,7 @@
         <v>3</v>
       </c>
       <c r="J59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K59">
         <v>0</v>
@@ -1956,7 +1963,7 @@
         <v>3</v>
       </c>
       <c r="J60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K60">
         <v>0</v>
@@ -2005,7 +2012,7 @@
         <v>4</v>
       </c>
       <c r="N62" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="O62">
         <v>14</v>
@@ -2025,7 +2032,7 @@
         <v>4</v>
       </c>
       <c r="N63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O63">
         <v>4</v>
@@ -2045,7 +2052,7 @@
         <v>4</v>
       </c>
       <c r="N64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O64">
         <v>1</v>
@@ -2065,7 +2072,7 @@
         <v>4</v>
       </c>
       <c r="N65" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O65">
         <v>5</v>
@@ -2085,7 +2092,7 @@
         <v>4</v>
       </c>
       <c r="N66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O66">
         <v>0</v>
@@ -2096,7 +2103,7 @@
         <v>4</v>
       </c>
       <c r="J67" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="K67">
         <v>14</v>
@@ -2105,7 +2112,7 @@
         <v>4</v>
       </c>
       <c r="N67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O67">
         <v>0</v>
@@ -2116,7 +2123,7 @@
         <v>4</v>
       </c>
       <c r="J68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K68">
         <v>4</v>
@@ -2125,7 +2132,7 @@
         <v>4</v>
       </c>
       <c r="N68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O68">
         <v>5</v>
@@ -2136,7 +2143,7 @@
         <v>4</v>
       </c>
       <c r="J69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K69">
         <v>1</v>
@@ -2145,7 +2152,7 @@
         <v>4</v>
       </c>
       <c r="N69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O69">
         <v>0</v>
@@ -2156,7 +2163,7 @@
         <v>4</v>
       </c>
       <c r="J70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K70">
         <v>5</v>
@@ -2165,7 +2172,7 @@
         <v>4</v>
       </c>
       <c r="N70" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O70">
         <v>6</v>
@@ -2176,7 +2183,7 @@
         <v>4</v>
       </c>
       <c r="J71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K71">
         <v>0</v>
@@ -2185,7 +2192,7 @@
         <v>4</v>
       </c>
       <c r="N71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O71">
         <v>4</v>
@@ -2196,7 +2203,7 @@
         <v>4</v>
       </c>
       <c r="J72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K72">
         <v>0</v>
@@ -2205,7 +2212,7 @@
         <v>4</v>
       </c>
       <c r="N72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O72">
         <v>2</v>
@@ -2216,7 +2223,7 @@
         <v>4</v>
       </c>
       <c r="J73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K73">
         <v>5</v>
@@ -2225,7 +2232,7 @@
         <v>4</v>
       </c>
       <c r="N73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O73">
         <v>0</v>
@@ -2236,7 +2243,7 @@
         <v>4</v>
       </c>
       <c r="J74" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K74">
         <v>0</v>
@@ -2247,7 +2254,7 @@
         <v>4</v>
       </c>
       <c r="J75" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K75">
         <v>6</v>
@@ -2258,7 +2265,7 @@
         <v>4</v>
       </c>
       <c r="J76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K76">
         <v>4</v>
@@ -2269,7 +2276,7 @@
         <v>4</v>
       </c>
       <c r="J77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K77">
         <v>2</v>
@@ -2280,7 +2287,7 @@
         <v>4</v>
       </c>
       <c r="J78" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K78">
         <v>0</v>

</xml_diff>

<commit_message>
nuevos graficos circulares, títulos, métricas y ajustes de vista en gráficas.
</commit_message>
<xml_diff>
--- a/app-medicine-r/modulos/data/datos_supensiones_por_especialidad.xlsx
+++ b/app-medicine-r/modulos/data/datos_supensiones_por_especialidad.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\app_health_r_medicine\app-mvp\modulos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\app_health_r_medicine\app-medicine-r\modulos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC20C13F-EEE4-4B87-BEA5-DF9F51169345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7DF454-EC23-4763-A019-CEAC10E4461F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{109DEA4C-15FF-477D-B494-C4225E7A906B}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>Urología</t>
   </si>
   <si>
-    <t>Cirugí digestiva alta</t>
-  </si>
-  <si>
     <t>Cirugía infantil</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>cantidad</t>
+  </si>
+  <si>
+    <t>cirugía digestiva alta</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="A1:O78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="L73" sqref="L73"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,22 +513,22 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
-        <v>27</v>
-      </c>
       <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" t="s">
         <v>29</v>
-      </c>
-      <c r="N1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -553,7 +553,7 @@
         <v/>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -586,7 +586,7 @@
         <v>68</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
         <v>1</v>
@@ -622,7 +622,7 @@
         <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
@@ -658,7 +658,7 @@
         <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
         <v>3</v>
@@ -694,7 +694,7 @@
         <v>30</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J6" t="s">
         <v>4</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>20</v>
@@ -775,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O8">
         <v>20</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>13</v>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O9">
         <v>13</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>12</v>
@@ -844,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O10">
         <v>12</v>
@@ -852,7 +852,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -880,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O11">
         <v>9</v>
@@ -888,7 +888,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -910,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O12">
         <v>4</v>
@@ -918,7 +918,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -934,7 +934,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K13">
         <v>20</v>
@@ -943,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O13">
         <v>4</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -967,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K14">
         <v>13</v>
@@ -976,7 +976,7 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O14">
         <v>3</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -997,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K15">
         <v>12</v>
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O15">
         <v>1</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <v>6</v>
@@ -1023,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K16">
         <v>9</v>
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1053,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K17">
         <v>4</v>
@@ -1062,7 +1062,7 @@
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -1083,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K18">
         <v>4</v>
@@ -1092,7 +1092,7 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1113,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K19">
         <v>3</v>
@@ -1122,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <f>SUM(B2:B19)</f>
@@ -1156,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -1176,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -1216,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -1236,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -1285,7 +1285,7 @@
         <v>2</v>
       </c>
       <c r="N26" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1305,7 +1305,7 @@
         <v>2</v>
       </c>
       <c r="N27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O27">
         <v>2</v>
@@ -1325,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="N28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O28">
         <v>0</v>
@@ -1345,7 +1345,7 @@
         <v>2</v>
       </c>
       <c r="N29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O29">
         <v>1</v>
@@ -1365,7 +1365,7 @@
         <v>2</v>
       </c>
       <c r="N30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O30">
         <v>0</v>
@@ -1376,7 +1376,7 @@
         <v>2</v>
       </c>
       <c r="J31" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -1385,7 +1385,7 @@
         <v>2</v>
       </c>
       <c r="N31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O31">
         <v>21</v>
@@ -1396,7 +1396,7 @@
         <v>2</v>
       </c>
       <c r="J32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K32">
         <v>2</v>
@@ -1405,7 +1405,7 @@
         <v>2</v>
       </c>
       <c r="N32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O32">
         <v>0</v>
@@ -1416,7 +1416,7 @@
         <v>2</v>
       </c>
       <c r="J33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -1425,7 +1425,7 @@
         <v>2</v>
       </c>
       <c r="N33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O33">
         <v>0</v>
@@ -1436,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="J34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K34">
         <v>1</v>
@@ -1445,7 +1445,7 @@
         <v>2</v>
       </c>
       <c r="N34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O34">
         <v>0</v>
@@ -1456,7 +1456,7 @@
         <v>2</v>
       </c>
       <c r="J35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -1465,7 +1465,7 @@
         <v>2</v>
       </c>
       <c r="N35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O35">
         <v>0</v>
@@ -1476,7 +1476,7 @@
         <v>2</v>
       </c>
       <c r="J36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K36">
         <v>21</v>
@@ -1485,7 +1485,7 @@
         <v>2</v>
       </c>
       <c r="N36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -1496,7 +1496,7 @@
         <v>2</v>
       </c>
       <c r="J37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -1505,7 +1505,7 @@
         <v>2</v>
       </c>
       <c r="N37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O37">
         <v>2</v>
@@ -1516,7 +1516,7 @@
         <v>2</v>
       </c>
       <c r="J38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -1536,7 +1536,7 @@
         <v>2</v>
       </c>
       <c r="J39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -1556,7 +1556,7 @@
         <v>2</v>
       </c>
       <c r="J40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -1576,7 +1576,7 @@
         <v>2</v>
       </c>
       <c r="J41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -1596,7 +1596,7 @@
         <v>2</v>
       </c>
       <c r="J42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K42">
         <v>2</v>
@@ -1645,7 +1645,7 @@
         <v>3</v>
       </c>
       <c r="N44" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O44">
         <v>2</v>
@@ -1665,7 +1665,7 @@
         <v>3</v>
       </c>
       <c r="N45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O45">
         <v>0</v>
@@ -1685,7 +1685,7 @@
         <v>3</v>
       </c>
       <c r="N46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -1705,7 +1705,7 @@
         <v>3</v>
       </c>
       <c r="N47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O47">
         <v>0</v>
@@ -1725,7 +1725,7 @@
         <v>3</v>
       </c>
       <c r="N48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O48">
         <v>0</v>
@@ -1736,7 +1736,7 @@
         <v>3</v>
       </c>
       <c r="J49" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K49">
         <v>2</v>
@@ -1745,7 +1745,7 @@
         <v>3</v>
       </c>
       <c r="N49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O49">
         <v>0</v>
@@ -1756,7 +1756,7 @@
         <v>3</v>
       </c>
       <c r="J50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K50">
         <v>0</v>
@@ -1765,7 +1765,7 @@
         <v>3</v>
       </c>
       <c r="N50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O50">
         <v>0</v>
@@ -1776,7 +1776,7 @@
         <v>3</v>
       </c>
       <c r="J51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K51">
         <v>0</v>
@@ -1785,7 +1785,7 @@
         <v>3</v>
       </c>
       <c r="N51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O51">
         <v>0</v>
@@ -1796,7 +1796,7 @@
         <v>3</v>
       </c>
       <c r="J52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K52">
         <v>0</v>
@@ -1805,7 +1805,7 @@
         <v>3</v>
       </c>
       <c r="N52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O52">
         <v>0</v>
@@ -1816,7 +1816,7 @@
         <v>3</v>
       </c>
       <c r="J53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -1825,7 +1825,7 @@
         <v>3</v>
       </c>
       <c r="N53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O53">
         <v>0</v>
@@ -1836,7 +1836,7 @@
         <v>3</v>
       </c>
       <c r="J54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K54">
         <v>0</v>
@@ -1845,7 +1845,7 @@
         <v>3</v>
       </c>
       <c r="N54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O54">
         <v>0</v>
@@ -1856,7 +1856,7 @@
         <v>3</v>
       </c>
       <c r="J55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K55">
         <v>0</v>
@@ -1865,7 +1865,7 @@
         <v>3</v>
       </c>
       <c r="N55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O55">
         <v>0</v>
@@ -1876,7 +1876,7 @@
         <v>3</v>
       </c>
       <c r="J56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K56">
         <v>0</v>
@@ -1896,7 +1896,7 @@
         <v>3</v>
       </c>
       <c r="J57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -1916,7 +1916,7 @@
         <v>3</v>
       </c>
       <c r="J58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K58">
         <v>0</v>
@@ -1936,7 +1936,7 @@
         <v>3</v>
       </c>
       <c r="J59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K59">
         <v>0</v>
@@ -1956,7 +1956,7 @@
         <v>3</v>
       </c>
       <c r="J60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K60">
         <v>0</v>
@@ -2005,7 +2005,7 @@
         <v>4</v>
       </c>
       <c r="N62" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O62">
         <v>14</v>
@@ -2025,7 +2025,7 @@
         <v>4</v>
       </c>
       <c r="N63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O63">
         <v>4</v>
@@ -2045,7 +2045,7 @@
         <v>4</v>
       </c>
       <c r="N64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O64">
         <v>1</v>
@@ -2065,7 +2065,7 @@
         <v>4</v>
       </c>
       <c r="N65" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O65">
         <v>5</v>
@@ -2085,7 +2085,7 @@
         <v>4</v>
       </c>
       <c r="N66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O66">
         <v>0</v>
@@ -2096,7 +2096,7 @@
         <v>4</v>
       </c>
       <c r="J67" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K67">
         <v>14</v>
@@ -2105,7 +2105,7 @@
         <v>4</v>
       </c>
       <c r="N67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O67">
         <v>0</v>
@@ -2116,7 +2116,7 @@
         <v>4</v>
       </c>
       <c r="J68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K68">
         <v>4</v>
@@ -2125,7 +2125,7 @@
         <v>4</v>
       </c>
       <c r="N68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O68">
         <v>5</v>
@@ -2136,7 +2136,7 @@
         <v>4</v>
       </c>
       <c r="J69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K69">
         <v>1</v>
@@ -2145,7 +2145,7 @@
         <v>4</v>
       </c>
       <c r="N69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O69">
         <v>0</v>
@@ -2156,7 +2156,7 @@
         <v>4</v>
       </c>
       <c r="J70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K70">
         <v>5</v>
@@ -2165,7 +2165,7 @@
         <v>4</v>
       </c>
       <c r="N70" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O70">
         <v>6</v>
@@ -2176,7 +2176,7 @@
         <v>4</v>
       </c>
       <c r="J71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K71">
         <v>0</v>
@@ -2185,7 +2185,7 @@
         <v>4</v>
       </c>
       <c r="N71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O71">
         <v>4</v>
@@ -2196,7 +2196,7 @@
         <v>4</v>
       </c>
       <c r="J72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K72">
         <v>0</v>
@@ -2205,7 +2205,7 @@
         <v>4</v>
       </c>
       <c r="N72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O72">
         <v>2</v>
@@ -2216,7 +2216,7 @@
         <v>4</v>
       </c>
       <c r="J73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K73">
         <v>5</v>
@@ -2225,7 +2225,7 @@
         <v>4</v>
       </c>
       <c r="N73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O73">
         <v>0</v>
@@ -2236,7 +2236,7 @@
         <v>4</v>
       </c>
       <c r="J74" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K74">
         <v>0</v>
@@ -2247,7 +2247,7 @@
         <v>4</v>
       </c>
       <c r="J75" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K75">
         <v>6</v>
@@ -2258,7 +2258,7 @@
         <v>4</v>
       </c>
       <c r="J76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K76">
         <v>4</v>
@@ -2269,7 +2269,7 @@
         <v>4</v>
       </c>
       <c r="J77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K77">
         <v>2</v>
@@ -2280,7 +2280,7 @@
         <v>4</v>
       </c>
       <c r="J78" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K78">
         <v>0</v>

</xml_diff>